<commit_message>
work on cases where the subtopic is the combination of two possible descriptions
</commit_message>
<xml_diff>
--- a/data/hierarchy/hierarchy_code.xlsx
+++ b/data/hierarchy/hierarchy_code.xlsx
@@ -1867,7 +1867,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Reserves (or residential)</t>
+          <t>Reserves</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1904,7 +1904,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Reserves (or residential)</t>
+          <t>Reserves</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Reserves (or residential)</t>
+          <t>Reserves</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -1978,7 +1978,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Reserves (or residential)</t>
+          <t>Reserves</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -2015,7 +2015,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Reserves (or residential)</t>
+          <t>Reserves</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -5345,7 +5345,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
@@ -5382,7 +5382,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
@@ -5419,7 +5419,7 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
@@ -5456,7 +5456,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
@@ -5493,7 +5493,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
@@ -5530,7 +5530,7 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
@@ -5567,7 +5567,7 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
@@ -5604,7 +5604,7 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
@@ -5641,7 +5641,7 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
@@ -5678,7 +5678,7 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
@@ -5715,7 +5715,7 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
@@ -5752,7 +5752,7 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
@@ -5789,7 +5789,7 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
@@ -5826,7 +5826,7 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
@@ -5863,7 +5863,7 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G147" t="inlineStr">
@@ -5900,7 +5900,7 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G148" t="inlineStr">
@@ -5937,7 +5937,7 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G149" t="inlineStr">
@@ -5974,7 +5974,7 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
@@ -6011,7 +6011,7 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G151" t="inlineStr">
@@ -6048,7 +6048,7 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
@@ -6085,7 +6085,7 @@
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G153" t="inlineStr">
@@ -8934,7 +8934,7 @@
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G230" t="inlineStr">
@@ -8971,7 +8971,7 @@
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G231" t="inlineStr">
@@ -9008,7 +9008,7 @@
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G232" t="inlineStr">
@@ -9045,7 +9045,7 @@
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G233" t="inlineStr">
@@ -9082,7 +9082,7 @@
       </c>
       <c r="F234" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G234" t="inlineStr">
@@ -9119,7 +9119,7 @@
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G235" t="inlineStr">
@@ -9156,7 +9156,7 @@
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G236" t="inlineStr">
@@ -9193,7 +9193,7 @@
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G237" t="inlineStr">
@@ -9230,7 +9230,7 @@
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G238" t="inlineStr">
@@ -9267,7 +9267,7 @@
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G239" t="inlineStr">
@@ -9304,7 +9304,7 @@
       </c>
       <c r="F240" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G240" t="inlineStr">
@@ -9341,7 +9341,7 @@
       </c>
       <c r="F241" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G241" t="inlineStr">
@@ -9378,7 +9378,7 @@
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G242" t="inlineStr">
@@ -10118,7 +10118,7 @@
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G262" t="inlineStr">
@@ -10155,7 +10155,7 @@
       </c>
       <c r="F263" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G263" t="inlineStr">
@@ -10192,7 +10192,7 @@
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G264" t="inlineStr">
@@ -13226,7 +13226,7 @@
       </c>
       <c r="F346" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G346" t="inlineStr">
@@ -13263,7 +13263,7 @@
       </c>
       <c r="F347" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G347" t="inlineStr">
@@ -16297,7 +16297,7 @@
       </c>
       <c r="F429" t="inlineStr">
         <is>
-          <t>Commitments (or compulsory)</t>
+          <t>Compulsory</t>
         </is>
       </c>
       <c r="G429" t="inlineStr">
@@ -19479,7 +19479,7 @@
       </c>
       <c r="F515" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G515" t="inlineStr">
@@ -19516,7 +19516,7 @@
       </c>
       <c r="F516" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Consumption</t>
         </is>
       </c>
       <c r="G516" t="inlineStr">
@@ -20589,7 +20589,7 @@
       </c>
       <c r="F545" t="inlineStr">
         <is>
-          <t>Atmosphere (or automated teller machine)</t>
+          <t>Atmosphere</t>
         </is>
       </c>
       <c r="G545" t="inlineStr">
@@ -20626,7 +20626,7 @@
       </c>
       <c r="F546" t="inlineStr">
         <is>
-          <t>Atmosphere (or automated teller machine)</t>
+          <t>Atmosphere</t>
         </is>
       </c>
       <c r="G546" t="inlineStr">
@@ -20663,7 +20663,7 @@
       </c>
       <c r="F547" t="inlineStr">
         <is>
-          <t>Atmosphere (or automated teller machine)</t>
+          <t>Atmosphere</t>
         </is>
       </c>
       <c r="G547" t="inlineStr">
@@ -20700,7 +20700,7 @@
       </c>
       <c r="F548" t="inlineStr">
         <is>
-          <t>Atmosphere (or automated teller machine)</t>
+          <t>Atmosphere</t>
         </is>
       </c>
       <c r="G548" t="inlineStr">
@@ -20737,7 +20737,7 @@
       </c>
       <c r="F549" t="inlineStr">
         <is>
-          <t>Atmosphere (or automated teller machine)</t>
+          <t>Atmosphere</t>
         </is>
       </c>
       <c r="G549" t="inlineStr">
@@ -24807,7 +24807,7 @@
       </c>
       <c r="F659" t="inlineStr">
         <is>
-          <t>Atmosphere (or automated teller machine)</t>
+          <t>Automated teller machines</t>
         </is>
       </c>
       <c r="G659" t="inlineStr">
@@ -25843,7 +25843,7 @@
       </c>
       <c r="F687" t="inlineStr">
         <is>
-          <t>Reserves (or residential)</t>
+          <t>Reserves</t>
         </is>
       </c>
       <c r="G687" t="inlineStr">
@@ -26107,7 +26107,7 @@
       </c>
       <c r="G694" t="inlineStr">
         <is>
-          <t>Transport receipts (or Turnover ratio)</t>
+          <t>Turnover ratio</t>
         </is>
       </c>
     </row>
@@ -27397,7 +27397,7 @@
       </c>
       <c r="F729" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Condom</t>
         </is>
       </c>
       <c r="G729" t="inlineStr">
@@ -27434,7 +27434,7 @@
       </c>
       <c r="F730" t="inlineStr">
         <is>
-          <t>Consumption (or condom)</t>
+          <t>Condom</t>
         </is>
       </c>
       <c r="G730" t="inlineStr">
@@ -30690,7 +30690,7 @@
       </c>
       <c r="F818" t="inlineStr">
         <is>
-          <t>Anemia (or animal)</t>
+          <t>Anemia</t>
         </is>
       </c>
       <c r="G818" t="inlineStr">
@@ -30727,7 +30727,7 @@
       </c>
       <c r="F819" t="inlineStr">
         <is>
-          <t>Anemia (or animal)</t>
+          <t>Anemia</t>
         </is>
       </c>
       <c r="G819" t="inlineStr">
@@ -30764,7 +30764,7 @@
       </c>
       <c r="F820" t="inlineStr">
         <is>
-          <t>Anemia (or animal)</t>
+          <t>Anemia</t>
         </is>
       </c>
       <c r="G820" t="inlineStr">
@@ -39903,7 +39903,7 @@
       </c>
       <c r="F1067" t="inlineStr">
         <is>
-          <t>Insolvency (or industry plus services)</t>
+          <t>Insolvency</t>
         </is>
       </c>
       <c r="G1067" t="inlineStr">
@@ -40088,7 +40088,7 @@
       </c>
       <c r="F1072" t="inlineStr">
         <is>
-          <t>Registration (or regulatory)</t>
+          <t xml:space="preserve">Registration </t>
         </is>
       </c>
       <c r="G1072" t="inlineStr">
@@ -40125,7 +40125,7 @@
       </c>
       <c r="F1073" t="inlineStr">
         <is>
-          <t>Registration (or regulatory)</t>
+          <t xml:space="preserve">Registration </t>
         </is>
       </c>
       <c r="G1073" t="inlineStr">
@@ -40162,7 +40162,7 @@
       </c>
       <c r="F1074" t="inlineStr">
         <is>
-          <t>Registration (or regulatory)</t>
+          <t xml:space="preserve">Registration </t>
         </is>
       </c>
       <c r="G1074" t="inlineStr">
@@ -40199,7 +40199,7 @@
       </c>
       <c r="F1075" t="inlineStr">
         <is>
-          <t>Registration (or regulatory)</t>
+          <t xml:space="preserve">Registration </t>
         </is>
       </c>
       <c r="G1075" t="inlineStr">
@@ -40236,7 +40236,7 @@
       </c>
       <c r="F1076" t="inlineStr">
         <is>
-          <t>Registration (or regulatory)</t>
+          <t xml:space="preserve">Registration </t>
         </is>
       </c>
       <c r="G1076" t="inlineStr">
@@ -40273,7 +40273,7 @@
       </c>
       <c r="F1077" t="inlineStr">
         <is>
-          <t>Registration (or regulatory)</t>
+          <t xml:space="preserve">Registration </t>
         </is>
       </c>
       <c r="G1077" t="inlineStr">
@@ -40310,7 +40310,7 @@
       </c>
       <c r="F1078" t="inlineStr">
         <is>
-          <t>Registration (or regulatory)</t>
+          <t xml:space="preserve">Registration </t>
         </is>
       </c>
       <c r="G1078" t="inlineStr">
@@ -40347,7 +40347,7 @@
       </c>
       <c r="F1079" t="inlineStr">
         <is>
-          <t>Registration (or regulatory)</t>
+          <t xml:space="preserve">Registration </t>
         </is>
       </c>
       <c r="G1079" t="inlineStr">
@@ -40384,7 +40384,7 @@
       </c>
       <c r="F1080" t="inlineStr">
         <is>
-          <t>Registration (or regulatory)</t>
+          <t xml:space="preserve">Registration </t>
         </is>
       </c>
       <c r="G1080" t="inlineStr">
@@ -40421,7 +40421,7 @@
       </c>
       <c r="F1081" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1081" t="inlineStr">
@@ -40458,7 +40458,7 @@
       </c>
       <c r="F1082" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1082" t="inlineStr">
@@ -40495,7 +40495,7 @@
       </c>
       <c r="F1083" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1083" t="inlineStr">
@@ -40532,7 +40532,7 @@
       </c>
       <c r="F1084" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1084" t="inlineStr">
@@ -40569,7 +40569,7 @@
       </c>
       <c r="F1085" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1085" t="inlineStr">
@@ -40606,7 +40606,7 @@
       </c>
       <c r="F1086" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1086" t="inlineStr">
@@ -40643,7 +40643,7 @@
       </c>
       <c r="F1087" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1087" t="inlineStr">
@@ -40680,7 +40680,7 @@
       </c>
       <c r="F1088" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1088" t="inlineStr">
@@ -42493,7 +42493,7 @@
       </c>
       <c r="F1137" t="inlineStr">
         <is>
-          <t>Private participation in infrastructure (or producer price index)</t>
+          <t>Private participation in infrastructure</t>
         </is>
       </c>
       <c r="G1137" t="inlineStr">
@@ -42530,7 +42530,7 @@
       </c>
       <c r="F1138" t="inlineStr">
         <is>
-          <t>Private participation in infrastructure (or producer price index)</t>
+          <t>Private participation in infrastructure</t>
         </is>
       </c>
       <c r="G1138" t="inlineStr">
@@ -42567,7 +42567,7 @@
       </c>
       <c r="F1139" t="inlineStr">
         <is>
-          <t>Private participation in infrastructure (or producer price index)</t>
+          <t>Private participation in infrastructure</t>
         </is>
       </c>
       <c r="G1139" t="inlineStr">
@@ -42604,7 +42604,7 @@
       </c>
       <c r="F1140" t="inlineStr">
         <is>
-          <t>Private participation in infrastructure (or producer price index)</t>
+          <t>Private participation in infrastructure</t>
         </is>
       </c>
       <c r="G1140" t="inlineStr">
@@ -43238,7 +43238,7 @@
       </c>
       <c r="G1157" t="inlineStr">
         <is>
-          <t>Infrastructure (or infant reported)</t>
+          <t>Infrastructure</t>
         </is>
       </c>
     </row>
@@ -43529,7 +43529,7 @@
       </c>
       <c r="F1165" t="inlineStr">
         <is>
-          <t>Interest payments (or international)</t>
+          <t>International</t>
         </is>
       </c>
       <c r="G1165" t="inlineStr">
@@ -43566,7 +43566,7 @@
       </c>
       <c r="F1166" t="inlineStr">
         <is>
-          <t>Interest payments (or international)</t>
+          <t>International</t>
         </is>
       </c>
       <c r="G1166" t="inlineStr">
@@ -43603,7 +43603,7 @@
       </c>
       <c r="F1167" t="inlineStr">
         <is>
-          <t>Interest payments (or international)</t>
+          <t>International</t>
         </is>
       </c>
       <c r="G1167" t="inlineStr">
@@ -43640,7 +43640,7 @@
       </c>
       <c r="F1168" t="inlineStr">
         <is>
-          <t>Interest payments (or international)</t>
+          <t>International</t>
         </is>
       </c>
       <c r="G1168" t="inlineStr">
@@ -43677,7 +43677,7 @@
       </c>
       <c r="F1169" t="inlineStr">
         <is>
-          <t>Interest payments (or international)</t>
+          <t>International</t>
         </is>
       </c>
       <c r="G1169" t="inlineStr">
@@ -43714,7 +43714,7 @@
       </c>
       <c r="F1170" t="inlineStr">
         <is>
-          <t>Interest payments (or international)</t>
+          <t>International</t>
         </is>
       </c>
       <c r="G1170" t="inlineStr">
@@ -43751,7 +43751,7 @@
       </c>
       <c r="F1171" t="inlineStr">
         <is>
-          <t>Interest payments (or international)</t>
+          <t>International</t>
         </is>
       </c>
       <c r="G1171" t="inlineStr">
@@ -43788,12 +43788,12 @@
       </c>
       <c r="F1172" t="inlineStr">
         <is>
-          <t>Interest payments (or international)</t>
+          <t>International</t>
         </is>
       </c>
       <c r="G1172" t="inlineStr">
         <is>
-          <t>Transport receipts (or Turnover ratio)</t>
+          <t>Transport receipts</t>
         </is>
       </c>
     </row>
@@ -43825,7 +43825,7 @@
       </c>
       <c r="F1173" t="inlineStr">
         <is>
-          <t>Interest payments (or international)</t>
+          <t>International</t>
         </is>
       </c>
       <c r="G1173" t="inlineStr">
@@ -43862,7 +43862,7 @@
       </c>
       <c r="F1174" t="inlineStr">
         <is>
-          <t>Interest payments (or international)</t>
+          <t>International</t>
         </is>
       </c>
       <c r="G1174" t="inlineStr">
@@ -45564,7 +45564,7 @@
       </c>
       <c r="F1220" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1220" t="inlineStr">
@@ -45601,7 +45601,7 @@
       </c>
       <c r="F1221" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1221" t="inlineStr">
@@ -45638,7 +45638,7 @@
       </c>
       <c r="F1222" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1222" t="inlineStr">
@@ -45675,7 +45675,7 @@
       </c>
       <c r="F1223" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1223" t="inlineStr">
@@ -45712,7 +45712,7 @@
       </c>
       <c r="F1224" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1224" t="inlineStr">
@@ -45749,7 +45749,7 @@
       </c>
       <c r="F1225" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1225" t="inlineStr">
@@ -45786,7 +45786,7 @@
       </c>
       <c r="F1226" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1226" t="inlineStr">
@@ -45823,7 +45823,7 @@
       </c>
       <c r="F1227" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1227" t="inlineStr">
@@ -45860,7 +45860,7 @@
       </c>
       <c r="F1228" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1228" t="inlineStr">
@@ -45897,7 +45897,7 @@
       </c>
       <c r="F1229" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1229" t="inlineStr">
@@ -45934,7 +45934,7 @@
       </c>
       <c r="F1230" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1230" t="inlineStr">
@@ -45971,7 +45971,7 @@
       </c>
       <c r="F1231" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1231" t="inlineStr">
@@ -46008,7 +46008,7 @@
       </c>
       <c r="F1232" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1232" t="inlineStr">
@@ -46045,7 +46045,7 @@
       </c>
       <c r="F1233" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1233" t="inlineStr">
@@ -46082,7 +46082,7 @@
       </c>
       <c r="F1234" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1234" t="inlineStr">
@@ -46119,7 +46119,7 @@
       </c>
       <c r="F1235" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tax revenue (or tax related)</t>
         </is>
       </c>
       <c r="G1235" t="inlineStr">
@@ -50226,7 +50226,7 @@
       </c>
       <c r="F1346" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G1346" t="inlineStr">
@@ -50263,7 +50263,7 @@
       </c>
       <c r="F1347" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G1347" t="inlineStr">
@@ -50300,7 +50300,7 @@
       </c>
       <c r="F1348" t="inlineStr">
         <is>
-          <t>Industry (or interest due) (or index)</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="G1348" t="inlineStr">
@@ -54752,12 +54752,12 @@
     <row r="1469">
       <c r="A1469" t="inlineStr">
         <is>
-          <t>TM.TAX.MRCH.BR.ZS</t>
+          <t>TX.QTY.MRCH.XD.WD</t>
         </is>
       </c>
       <c r="B1469" t="inlineStr">
         <is>
-          <t>Bound rate, simple mean, all products (%)</t>
+          <t>Export volume index (2015 = 100)</t>
         </is>
       </c>
       <c r="C1469" t="inlineStr">
@@ -54772,12 +54772,12 @@
       </c>
       <c r="E1469" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Exports</t>
         </is>
       </c>
       <c r="F1469" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Quantity (volume)</t>
         </is>
       </c>
       <c r="G1469" t="inlineStr">
@@ -54789,12 +54789,12 @@
     <row r="1470">
       <c r="A1470" t="inlineStr">
         <is>
-          <t>TM.TAX.MRCH.BC.ZS</t>
+          <t>TX.VAL.MRCH.XD.WD</t>
         </is>
       </c>
       <c r="B1470" t="inlineStr">
         <is>
-          <t>Binding coverage, all products (%)</t>
+          <t>Export value index (2015 = 100)</t>
         </is>
       </c>
       <c r="C1470" t="inlineStr">
@@ -54809,12 +54809,12 @@
       </c>
       <c r="E1470" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Exports</t>
         </is>
       </c>
       <c r="F1470" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Value</t>
         </is>
       </c>
       <c r="G1470" t="inlineStr">
@@ -54826,12 +54826,12 @@
     <row r="1471">
       <c r="A1471" t="inlineStr">
         <is>
-          <t>TM.TAX.MRCH.WM.FN.ZS</t>
+          <t>TM.QTY.MRCH.XD.WD</t>
         </is>
       </c>
       <c r="B1471" t="inlineStr">
         <is>
-          <t>Tariff rate, most favored nation, weighted mean, all products (%)</t>
+          <t>Import volume index (2015 = 100)</t>
         </is>
       </c>
       <c r="C1471" t="inlineStr">
@@ -54846,12 +54846,12 @@
       </c>
       <c r="E1471" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1471" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Quantity (volume)</t>
         </is>
       </c>
       <c r="G1471" t="inlineStr">
@@ -54863,12 +54863,12 @@
     <row r="1472">
       <c r="A1472" t="inlineStr">
         <is>
-          <t>TM.TAX.MRCH.IP.ZS</t>
+          <t>TM.TAX.MRCH.BR.ZS</t>
         </is>
       </c>
       <c r="B1472" t="inlineStr">
         <is>
-          <t>Share of tariff lines with international peaks, all products (%)</t>
+          <t>Bound rate, simple mean, all products (%)</t>
         </is>
       </c>
       <c r="C1472" t="inlineStr">
@@ -54883,12 +54883,12 @@
       </c>
       <c r="E1472" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1472" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1472" t="inlineStr">
@@ -54900,12 +54900,12 @@
     <row r="1473">
       <c r="A1473" t="inlineStr">
         <is>
-          <t>TM.TAX.MRCH.WM.AR.ZS</t>
+          <t>TM.TAX.MRCH.BC.ZS</t>
         </is>
       </c>
       <c r="B1473" t="inlineStr">
         <is>
-          <t>Tariff rate, applied, weighted mean, all products (%)</t>
+          <t>Binding coverage, all products (%)</t>
         </is>
       </c>
       <c r="C1473" t="inlineStr">
@@ -54920,12 +54920,12 @@
       </c>
       <c r="E1473" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1473" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1473" t="inlineStr">
@@ -54937,12 +54937,12 @@
     <row r="1474">
       <c r="A1474" t="inlineStr">
         <is>
-          <t>TM.TAX.MRCH.SM.AR.ZS</t>
+          <t>TM.TAX.MRCH.WM.FN.ZS</t>
         </is>
       </c>
       <c r="B1474" t="inlineStr">
         <is>
-          <t>Tariff rate, applied, simple mean, all products (%)</t>
+          <t>Tariff rate, most favored nation, weighted mean, all products (%)</t>
         </is>
       </c>
       <c r="C1474" t="inlineStr">
@@ -54957,12 +54957,12 @@
       </c>
       <c r="E1474" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1474" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1474" t="inlineStr">
@@ -54974,12 +54974,12 @@
     <row r="1475">
       <c r="A1475" t="inlineStr">
         <is>
-          <t>TM.TAX.MRCH.SR.ZS</t>
+          <t>TM.TAX.MRCH.IP.ZS</t>
         </is>
       </c>
       <c r="B1475" t="inlineStr">
         <is>
-          <t>Share of tariff lines with specific rates, all products (%)</t>
+          <t>Share of tariff lines with international peaks, all products (%)</t>
         </is>
       </c>
       <c r="C1475" t="inlineStr">
@@ -54994,12 +54994,12 @@
       </c>
       <c r="E1475" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1475" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1475" t="inlineStr">
@@ -55011,12 +55011,12 @@
     <row r="1476">
       <c r="A1476" t="inlineStr">
         <is>
-          <t>TM.TAX.MRCH.SM.FN.ZS</t>
+          <t>TM.TAX.MRCH.WM.AR.ZS</t>
         </is>
       </c>
       <c r="B1476" t="inlineStr">
         <is>
-          <t>Tariff rate, most favored nation, simple mean, all products (%)</t>
+          <t>Tariff rate, applied, weighted mean, all products (%)</t>
         </is>
       </c>
       <c r="C1476" t="inlineStr">
@@ -55031,12 +55031,12 @@
       </c>
       <c r="E1476" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1476" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1476" t="inlineStr">
@@ -55048,12 +55048,12 @@
     <row r="1477">
       <c r="A1477" t="inlineStr">
         <is>
-          <t>TM.TAX.MANF.IP.ZS</t>
+          <t>TM.TAX.MRCH.SM.AR.ZS</t>
         </is>
       </c>
       <c r="B1477" t="inlineStr">
         <is>
-          <t>Share of tariff lines with international peaks, manufactured products (%)</t>
+          <t>Tariff rate, applied, simple mean, all products (%)</t>
         </is>
       </c>
       <c r="C1477" t="inlineStr">
@@ -55068,29 +55068,29 @@
       </c>
       <c r="E1477" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1477" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1477" t="inlineStr">
         <is>
-          <t>Manufacturing</t>
+          <t>Goods (merchandise)</t>
         </is>
       </c>
     </row>
     <row r="1478">
       <c r="A1478" t="inlineStr">
         <is>
-          <t>TM.TAX.MANF.BC.ZS</t>
+          <t>TM.TAX.MRCH.SR.ZS</t>
         </is>
       </c>
       <c r="B1478" t="inlineStr">
         <is>
-          <t>Binding coverage, manufactured products (%)</t>
+          <t>Share of tariff lines with specific rates, all products (%)</t>
         </is>
       </c>
       <c r="C1478" t="inlineStr">
@@ -55105,29 +55105,29 @@
       </c>
       <c r="E1478" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1478" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1478" t="inlineStr">
         <is>
-          <t>Manufacturing</t>
+          <t>Goods (merchandise)</t>
         </is>
       </c>
     </row>
     <row r="1479">
       <c r="A1479" t="inlineStr">
         <is>
-          <t>TM.TAX.MANF.WM.FN.ZS</t>
+          <t>TM.TAX.MRCH.SM.FN.ZS</t>
         </is>
       </c>
       <c r="B1479" t="inlineStr">
         <is>
-          <t>Tariff rate, most favored nation, weighted mean, manufactured products (%)</t>
+          <t>Tariff rate, most favored nation, simple mean, all products (%)</t>
         </is>
       </c>
       <c r="C1479" t="inlineStr">
@@ -55142,29 +55142,29 @@
       </c>
       <c r="E1479" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1479" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1479" t="inlineStr">
         <is>
-          <t>Manufacturing</t>
+          <t>Goods (merchandise)</t>
         </is>
       </c>
     </row>
     <row r="1480">
       <c r="A1480" t="inlineStr">
         <is>
-          <t>TM.TAX.MANF.SM.FN.ZS</t>
+          <t>TM.TAX.MANF.IP.ZS</t>
         </is>
       </c>
       <c r="B1480" t="inlineStr">
         <is>
-          <t>Tariff rate, most favored nation, simple mean, manufactured products (%)</t>
+          <t>Share of tariff lines with international peaks, manufactured products (%)</t>
         </is>
       </c>
       <c r="C1480" t="inlineStr">
@@ -55179,12 +55179,12 @@
       </c>
       <c r="E1480" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1480" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1480" t="inlineStr">
@@ -55196,12 +55196,12 @@
     <row r="1481">
       <c r="A1481" t="inlineStr">
         <is>
-          <t>TM.TAX.MANF.WM.AR.ZS</t>
+          <t>TM.TAX.MANF.BC.ZS</t>
         </is>
       </c>
       <c r="B1481" t="inlineStr">
         <is>
-          <t>Tariff rate, applied, weighted mean, manufactured products (%)</t>
+          <t>Binding coverage, manufactured products (%)</t>
         </is>
       </c>
       <c r="C1481" t="inlineStr">
@@ -55216,12 +55216,12 @@
       </c>
       <c r="E1481" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1481" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1481" t="inlineStr">
@@ -55233,12 +55233,12 @@
     <row r="1482">
       <c r="A1482" t="inlineStr">
         <is>
-          <t>TM.TAX.MANF.SM.AR.ZS</t>
+          <t>TM.TAX.MANF.WM.FN.ZS</t>
         </is>
       </c>
       <c r="B1482" t="inlineStr">
         <is>
-          <t>Tariff rate, applied, simple mean, manufactured products (%)</t>
+          <t>Tariff rate, most favored nation, weighted mean, manufactured products (%)</t>
         </is>
       </c>
       <c r="C1482" t="inlineStr">
@@ -55253,12 +55253,12 @@
       </c>
       <c r="E1482" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1482" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1482" t="inlineStr">
@@ -55270,12 +55270,12 @@
     <row r="1483">
       <c r="A1483" t="inlineStr">
         <is>
-          <t>TM.TAX.MANF.BR.ZS</t>
+          <t>TM.TAX.MANF.SM.FN.ZS</t>
         </is>
       </c>
       <c r="B1483" t="inlineStr">
         <is>
-          <t>Bound rate, simple mean, manufactured products (%)</t>
+          <t>Tariff rate, most favored nation, simple mean, manufactured products (%)</t>
         </is>
       </c>
       <c r="C1483" t="inlineStr">
@@ -55290,12 +55290,12 @@
       </c>
       <c r="E1483" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1483" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1483" t="inlineStr">
@@ -55307,12 +55307,12 @@
     <row r="1484">
       <c r="A1484" t="inlineStr">
         <is>
-          <t>TM.TAX.MANF.SR.ZS</t>
+          <t>TM.TAX.MANF.WM.AR.ZS</t>
         </is>
       </c>
       <c r="B1484" t="inlineStr">
         <is>
-          <t>Share of tariff lines with specific rates, manufactured products (%)</t>
+          <t>Tariff rate, applied, weighted mean, manufactured products (%)</t>
         </is>
       </c>
       <c r="C1484" t="inlineStr">
@@ -55327,12 +55327,12 @@
       </c>
       <c r="E1484" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1484" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1484" t="inlineStr">
@@ -55344,12 +55344,12 @@
     <row r="1485">
       <c r="A1485" t="inlineStr">
         <is>
-          <t>TM.TAX.TCOM.BR.ZS</t>
+          <t>TM.TAX.MANF.SM.AR.ZS</t>
         </is>
       </c>
       <c r="B1485" t="inlineStr">
         <is>
-          <t>Bound rate, simple mean, primary products (%)</t>
+          <t>Tariff rate, applied, simple mean, manufactured products (%)</t>
         </is>
       </c>
       <c r="C1485" t="inlineStr">
@@ -55364,29 +55364,29 @@
       </c>
       <c r="E1485" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1485" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1485" t="inlineStr">
         <is>
-          <t>Primary products (commodities)</t>
+          <t>Manufacturing</t>
         </is>
       </c>
     </row>
     <row r="1486">
       <c r="A1486" t="inlineStr">
         <is>
-          <t>TM.TAX.TCOM.WM.FN.ZS</t>
+          <t>TM.TAX.MANF.BR.ZS</t>
         </is>
       </c>
       <c r="B1486" t="inlineStr">
         <is>
-          <t>Tariff rate, most favored nation, weighted mean, primary products (%)</t>
+          <t>Bound rate, simple mean, manufactured products (%)</t>
         </is>
       </c>
       <c r="C1486" t="inlineStr">
@@ -55401,29 +55401,29 @@
       </c>
       <c r="E1486" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1486" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1486" t="inlineStr">
         <is>
-          <t>Primary products (commodities)</t>
+          <t>Manufacturing</t>
         </is>
       </c>
     </row>
     <row r="1487">
       <c r="A1487" t="inlineStr">
         <is>
-          <t>TM.TAX.TCOM.BC.ZS</t>
+          <t>TM.TAX.MANF.SR.ZS</t>
         </is>
       </c>
       <c r="B1487" t="inlineStr">
         <is>
-          <t>Binding coverage, primary products (%)</t>
+          <t>Share of tariff lines with specific rates, manufactured products (%)</t>
         </is>
       </c>
       <c r="C1487" t="inlineStr">
@@ -55438,29 +55438,29 @@
       </c>
       <c r="E1487" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1487" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1487" t="inlineStr">
         <is>
-          <t>Primary products (commodities)</t>
+          <t>Manufacturing</t>
         </is>
       </c>
     </row>
     <row r="1488">
       <c r="A1488" t="inlineStr">
         <is>
-          <t>TM.TAX.TCOM.SM.FN.ZS</t>
+          <t>TM.TAX.TCOM.BR.ZS</t>
         </is>
       </c>
       <c r="B1488" t="inlineStr">
         <is>
-          <t>Tariff rate, most favored nation, simple mean, primary products (%)</t>
+          <t>Bound rate, simple mean, primary products (%)</t>
         </is>
       </c>
       <c r="C1488" t="inlineStr">
@@ -55475,12 +55475,12 @@
       </c>
       <c r="E1488" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1488" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1488" t="inlineStr">
@@ -55492,12 +55492,12 @@
     <row r="1489">
       <c r="A1489" t="inlineStr">
         <is>
-          <t>TM.TAX.TCOM.WM.AR.ZS</t>
+          <t>TM.TAX.TCOM.WM.FN.ZS</t>
         </is>
       </c>
       <c r="B1489" t="inlineStr">
         <is>
-          <t>Tariff rate, applied, weighted mean, primary products (%)</t>
+          <t>Tariff rate, most favored nation, weighted mean, primary products (%)</t>
         </is>
       </c>
       <c r="C1489" t="inlineStr">
@@ -55512,12 +55512,12 @@
       </c>
       <c r="E1489" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1489" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1489" t="inlineStr">
@@ -55529,12 +55529,12 @@
     <row r="1490">
       <c r="A1490" t="inlineStr">
         <is>
-          <t>TM.TAX.TCOM.SM.AR.ZS</t>
+          <t>TM.TAX.TCOM.BC.ZS</t>
         </is>
       </c>
       <c r="B1490" t="inlineStr">
         <is>
-          <t>Tariff rate, applied, simple mean, primary products (%)</t>
+          <t>Binding coverage, primary products (%)</t>
         </is>
       </c>
       <c r="C1490" t="inlineStr">
@@ -55549,12 +55549,12 @@
       </c>
       <c r="E1490" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1490" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1490" t="inlineStr">
@@ -55566,12 +55566,12 @@
     <row r="1491">
       <c r="A1491" t="inlineStr">
         <is>
-          <t>TM.TAX.TCOM.SR.ZS</t>
+          <t>TM.TAX.TCOM.SM.FN.ZS</t>
         </is>
       </c>
       <c r="B1491" t="inlineStr">
         <is>
-          <t>Share of tariff lines with specific rates, primary products (%)</t>
+          <t>Tariff rate, most favored nation, simple mean, primary products (%)</t>
         </is>
       </c>
       <c r="C1491" t="inlineStr">
@@ -55586,12 +55586,12 @@
       </c>
       <c r="E1491" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1491" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1491" t="inlineStr">
@@ -55603,12 +55603,12 @@
     <row r="1492">
       <c r="A1492" t="inlineStr">
         <is>
-          <t>TM.TAX.TCOM.IP.ZS</t>
+          <t>TM.TAX.TCOM.WM.AR.ZS</t>
         </is>
       </c>
       <c r="B1492" t="inlineStr">
         <is>
-          <t>Share of tariff lines with international peaks, primary products (%)</t>
+          <t>Tariff rate, applied, weighted mean, primary products (%)</t>
         </is>
       </c>
       <c r="C1492" t="inlineStr">
@@ -55623,12 +55623,12 @@
       </c>
       <c r="E1492" t="inlineStr">
         <is>
-          <t>Tariffs</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1492" t="inlineStr">
         <is>
-          <t>Tax revenue (or tariff) (or tax related)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1492" t="inlineStr">
@@ -55640,12 +55640,12 @@
     <row r="1493">
       <c r="A1493" t="inlineStr">
         <is>
-          <t>TT.PRI.MRCH.XD.WD</t>
+          <t>TM.TAX.TCOM.SM.AR.ZS</t>
         </is>
       </c>
       <c r="B1493" t="inlineStr">
         <is>
-          <t>Net barter terms of trade index (2015 = 100)</t>
+          <t>Tariff rate, applied, simple mean, primary products (%)</t>
         </is>
       </c>
       <c r="C1493" t="inlineStr">
@@ -55660,29 +55660,29 @@
       </c>
       <c r="E1493" t="inlineStr">
         <is>
-          <t>Trade indexes</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1493" t="inlineStr">
         <is>
-          <t>Price</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1493" t="inlineStr">
         <is>
-          <t>Goods (merchandise)</t>
+          <t>Primary products (commodities)</t>
         </is>
       </c>
     </row>
     <row r="1494">
       <c r="A1494" t="inlineStr">
         <is>
-          <t>TX.QTY.MRCH.XD.WD</t>
+          <t>TM.TAX.TCOM.SR.ZS</t>
         </is>
       </c>
       <c r="B1494" t="inlineStr">
         <is>
-          <t>Export volume index (2015 = 100)</t>
+          <t>Share of tariff lines with specific rates, primary products (%)</t>
         </is>
       </c>
       <c r="C1494" t="inlineStr">
@@ -55697,29 +55697,29 @@
       </c>
       <c r="E1494" t="inlineStr">
         <is>
-          <t>Trade indexes</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1494" t="inlineStr">
         <is>
-          <t>Quantity (volume)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1494" t="inlineStr">
         <is>
-          <t>Goods (merchandise)</t>
+          <t>Primary products (commodities)</t>
         </is>
       </c>
     </row>
     <row r="1495">
       <c r="A1495" t="inlineStr">
         <is>
-          <t>TM.QTY.MRCH.XD.WD</t>
+          <t>TM.TAX.TCOM.IP.ZS</t>
         </is>
       </c>
       <c r="B1495" t="inlineStr">
         <is>
-          <t>Import volume index (2015 = 100)</t>
+          <t>Share of tariff lines with international peaks, primary products (%)</t>
         </is>
       </c>
       <c r="C1495" t="inlineStr">
@@ -55734,17 +55734,17 @@
       </c>
       <c r="E1495" t="inlineStr">
         <is>
-          <t>Trade indexes</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1495" t="inlineStr">
         <is>
-          <t>Quantity (volume)</t>
+          <t>Tariff</t>
         </is>
       </c>
       <c r="G1495" t="inlineStr">
         <is>
-          <t>Goods (merchandise)</t>
+          <t>Primary products (commodities)</t>
         </is>
       </c>
     </row>
@@ -55771,7 +55771,7 @@
       </c>
       <c r="E1496" t="inlineStr">
         <is>
-          <t>Trade indexes</t>
+          <t>Imports</t>
         </is>
       </c>
       <c r="F1496" t="inlineStr">
@@ -55788,12 +55788,12 @@
     <row r="1497">
       <c r="A1497" t="inlineStr">
         <is>
-          <t>TX.VAL.MRCH.XD.WD</t>
+          <t>TT.PRI.MRCH.XD.WD</t>
         </is>
       </c>
       <c r="B1497" t="inlineStr">
         <is>
-          <t>Export value index (2015 = 100)</t>
+          <t>Net barter terms of trade index (2015 = 100)</t>
         </is>
       </c>
       <c r="C1497" t="inlineStr">
@@ -55808,12 +55808,12 @@
       </c>
       <c r="E1497" t="inlineStr">
         <is>
-          <t>Trade indexes</t>
+          <t>Terms of trade</t>
         </is>
       </c>
       <c r="F1497" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>Price</t>
         </is>
       </c>
       <c r="G1497" t="inlineStr">

</xml_diff>

<commit_message>
change some values (personal)
</commit_message>
<xml_diff>
--- a/data/hierarchy/hierarchy_code.xlsx
+++ b/data/hierarchy/hierarchy_code.xlsx
@@ -16013,12 +16013,12 @@
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>SE.ADT.1524.LT.FE.ZS</t>
+          <t>SE.COM.DURS</t>
         </is>
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>Literacy rate, youth female (% of females ages 15-24)</t>
+          <t>Compulsory education, duration (years)</t>
         </is>
       </c>
       <c r="C422" t="inlineStr">
@@ -16038,24 +16038,24 @@
       </c>
       <c r="F422" t="inlineStr">
         <is>
-          <t>Adult</t>
+          <t>Compulsory</t>
         </is>
       </c>
       <c r="G422" t="inlineStr">
         <is>
-          <t>Age 15-24</t>
+          <t>Duration</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>SE.ADT.1524.LT.FM.ZS</t>
+          <t>SE.LPV.PRIM.MA</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>Literacy rate, youth (ages 15-24), gender parity index (GPI)</t>
+          <t>Learning poverty: Share of Male Children at the End-of-Primary age below minimum reading proficiency adjusted by Out-of-School Children (%)</t>
         </is>
       </c>
       <c r="C423" t="inlineStr">
@@ -16075,24 +16075,24 @@
       </c>
       <c r="F423" t="inlineStr">
         <is>
-          <t>Adult</t>
+          <t>Learning poverty</t>
         </is>
       </c>
       <c r="G423" t="inlineStr">
         <is>
-          <t>Age 15-24</t>
+          <t>Primary education</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>SE.ADT.1524.LT.MA.ZS</t>
+          <t>SE.LPV.PRIM.FE</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>Literacy rate, youth male (% of males ages 15-24)</t>
+          <t>Learning poverty: Share of Female Children at the End-of-Primary age below minimum reading proficiency adjusted by Out-of-School Children (%)</t>
         </is>
       </c>
       <c r="C424" t="inlineStr">
@@ -16112,24 +16112,24 @@
       </c>
       <c r="F424" t="inlineStr">
         <is>
-          <t>Adult</t>
+          <t>Learning poverty</t>
         </is>
       </c>
       <c r="G424" t="inlineStr">
         <is>
-          <t>Age 15-24</t>
+          <t>Primary education</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>SE.ADT.1524.LT.ZS</t>
+          <t>SE.LPV.PRIM</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>Literacy rate, youth total (% of people ages 15-24)</t>
+          <t>Learning poverty: Share of Children at the End-of-Primary age below minimum reading proficiency adjusted by Out-of-School Children (%)</t>
         </is>
       </c>
       <c r="C425" t="inlineStr">
@@ -16149,24 +16149,24 @@
       </c>
       <c r="F425" t="inlineStr">
         <is>
-          <t>Adult</t>
+          <t>Learning poverty</t>
         </is>
       </c>
       <c r="G425" t="inlineStr">
         <is>
-          <t>Age 15-24</t>
+          <t>Primary education</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>SE.ADT.LITR.ZS</t>
+          <t>SE.LPV.PRIM.LD.FE</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>Literacy rate, adult total (% of people ages 15 and above)</t>
+          <t>Female pupils below minimum reading proficiency at end of primary (%). Low GAML threshold</t>
         </is>
       </c>
       <c r="C426" t="inlineStr">
@@ -16186,24 +16186,24 @@
       </c>
       <c r="F426" t="inlineStr">
         <is>
-          <t>Adult</t>
+          <t>Learning poverty</t>
         </is>
       </c>
       <c r="G426" t="inlineStr">
         <is>
-          <t>Literacy</t>
+          <t>Primary education</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>SE.ADT.LITR.MA.ZS</t>
+          <t>SE.LPV.PRIM.SD.FE</t>
         </is>
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>Literacy rate, adult male (% of males ages 15 and above)</t>
+          <t>Female primary school age children out-of-school (%)</t>
         </is>
       </c>
       <c r="C427" t="inlineStr">
@@ -16223,24 +16223,24 @@
       </c>
       <c r="F427" t="inlineStr">
         <is>
-          <t>Adult</t>
+          <t>Learning poverty</t>
         </is>
       </c>
       <c r="G427" t="inlineStr">
         <is>
-          <t>Literacy</t>
+          <t>Primary education</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>SE.ADT.LITR.FE.ZS</t>
+          <t>SE.LPV.PRIM.LD</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>Literacy rate, adult female (% of females ages 15 and above)</t>
+          <t>Pupils below minimum reading proficiency at end of primary (%). Low GAML threshold</t>
         </is>
       </c>
       <c r="C428" t="inlineStr">
@@ -16260,24 +16260,24 @@
       </c>
       <c r="F428" t="inlineStr">
         <is>
-          <t>Adult</t>
+          <t>Learning poverty</t>
         </is>
       </c>
       <c r="G428" t="inlineStr">
         <is>
-          <t>Literacy</t>
+          <t>Primary education</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>SE.COM.DURS</t>
+          <t>SE.LPV.PRIM.SD</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>Compulsory education, duration (years)</t>
+          <t>Primary school age children out-of-school (%)</t>
         </is>
       </c>
       <c r="C429" t="inlineStr">
@@ -16297,24 +16297,24 @@
       </c>
       <c r="F429" t="inlineStr">
         <is>
-          <t>Compulsory</t>
+          <t>Learning poverty</t>
         </is>
       </c>
       <c r="G429" t="inlineStr">
         <is>
-          <t>Duration</t>
+          <t>Primary education</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>SE.LPV.PRIM.MA</t>
+          <t>SE.LPV.PRIM.LD.MA</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>Learning poverty: Share of Male Children at the End-of-Primary age below minimum reading proficiency adjusted by Out-of-School Children (%)</t>
+          <t>Male pupils below minimum reading proficiency at end of primary (%). Low GAML threshold</t>
         </is>
       </c>
       <c r="C430" t="inlineStr">
@@ -16334,7 +16334,7 @@
       </c>
       <c r="F430" t="inlineStr">
         <is>
-          <t>Low Poverty Vulnerability</t>
+          <t>Learning poverty</t>
         </is>
       </c>
       <c r="G430" t="inlineStr">
@@ -16346,12 +16346,12 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>SE.LPV.PRIM.FE</t>
+          <t>SE.LPV.PRIM.SD.MA</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>Learning poverty: Share of Female Children at the End-of-Primary age below minimum reading proficiency adjusted by Out-of-School Children (%)</t>
+          <t>Male primary school age children out-of-school (%)</t>
         </is>
       </c>
       <c r="C431" t="inlineStr">
@@ -16371,7 +16371,7 @@
       </c>
       <c r="F431" t="inlineStr">
         <is>
-          <t>Low Poverty Vulnerability</t>
+          <t>Learning poverty</t>
         </is>
       </c>
       <c r="G431" t="inlineStr">
@@ -16383,12 +16383,12 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>SE.LPV.PRIM</t>
+          <t>SE.ADT.LITR.ZS</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>Learning poverty: Share of Children at the End-of-Primary age below minimum reading proficiency adjusted by Out-of-School Children (%)</t>
+          <t>Literacy rate, adult total (% of people ages 15 and above)</t>
         </is>
       </c>
       <c r="C432" t="inlineStr">
@@ -16408,24 +16408,24 @@
       </c>
       <c r="F432" t="inlineStr">
         <is>
-          <t>Low Poverty Vulnerability</t>
+          <t>Literacy rate</t>
         </is>
       </c>
       <c r="G432" t="inlineStr">
         <is>
-          <t>Primary education</t>
+          <t>Adult (ages 15 and above)</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>SE.LPV.PRIM.LD.FE</t>
+          <t>SE.ADT.LITR.MA.ZS</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>Female pupils below minimum reading proficiency at end of primary (%). Low GAML threshold</t>
+          <t>Literacy rate, adult male (% of males ages 15 and above)</t>
         </is>
       </c>
       <c r="C433" t="inlineStr">
@@ -16445,24 +16445,24 @@
       </c>
       <c r="F433" t="inlineStr">
         <is>
-          <t>Low Poverty Vulnerability</t>
+          <t>Literacy rate</t>
         </is>
       </c>
       <c r="G433" t="inlineStr">
         <is>
-          <t>Primary education</t>
+          <t>Adult (ages 15 and above)</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>SE.LPV.PRIM.SD.FE</t>
+          <t>SE.ADT.LITR.FE.ZS</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>Female primary school age children out-of-school (%)</t>
+          <t>Literacy rate, adult female (% of females ages 15 and above)</t>
         </is>
       </c>
       <c r="C434" t="inlineStr">
@@ -16482,24 +16482,24 @@
       </c>
       <c r="F434" t="inlineStr">
         <is>
-          <t>Low Poverty Vulnerability</t>
+          <t>Literacy rate</t>
         </is>
       </c>
       <c r="G434" t="inlineStr">
         <is>
-          <t>Primary education</t>
+          <t>Adult (ages 15 and above)</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>SE.LPV.PRIM.LD</t>
+          <t>SE.ADT.1524.LT.FE.ZS</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>Pupils below minimum reading proficiency at end of primary (%). Low GAML threshold</t>
+          <t>Literacy rate, youth female (% of females ages 15-24)</t>
         </is>
       </c>
       <c r="C435" t="inlineStr">
@@ -16519,24 +16519,24 @@
       </c>
       <c r="F435" t="inlineStr">
         <is>
-          <t>Low Poverty Vulnerability</t>
+          <t>Literacy rate</t>
         </is>
       </c>
       <c r="G435" t="inlineStr">
         <is>
-          <t>Primary education</t>
+          <t>Youth (ages 15-24)</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>SE.LPV.PRIM.SD</t>
+          <t>SE.ADT.1524.LT.FM.ZS</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>Primary school age children out-of-school (%)</t>
+          <t>Literacy rate, youth (ages 15-24), gender parity index (GPI)</t>
         </is>
       </c>
       <c r="C436" t="inlineStr">
@@ -16556,24 +16556,24 @@
       </c>
       <c r="F436" t="inlineStr">
         <is>
-          <t>Low Poverty Vulnerability</t>
+          <t>Literacy rate</t>
         </is>
       </c>
       <c r="G436" t="inlineStr">
         <is>
-          <t>Primary education</t>
+          <t>Youth (ages 15-24)</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>SE.LPV.PRIM.LD.MA</t>
+          <t>SE.ADT.1524.LT.MA.ZS</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>Male pupils below minimum reading proficiency at end of primary (%). Low GAML threshold</t>
+          <t>Literacy rate, youth male (% of males ages 15-24)</t>
         </is>
       </c>
       <c r="C437" t="inlineStr">
@@ -16593,24 +16593,24 @@
       </c>
       <c r="F437" t="inlineStr">
         <is>
-          <t>Low Poverty Vulnerability</t>
+          <t>Literacy rate</t>
         </is>
       </c>
       <c r="G437" t="inlineStr">
         <is>
-          <t>Primary education</t>
+          <t>Youth (ages 15-24)</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>SE.LPV.PRIM.SD.MA</t>
+          <t>SE.ADT.1524.LT.ZS</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>Male primary school age children out-of-school (%)</t>
+          <t>Literacy rate, youth total (% of people ages 15-24)</t>
         </is>
       </c>
       <c r="C438" t="inlineStr">
@@ -16630,12 +16630,12 @@
       </c>
       <c r="F438" t="inlineStr">
         <is>
-          <t>Low Poverty Vulnerability</t>
+          <t>Literacy rate</t>
         </is>
       </c>
       <c r="G438" t="inlineStr">
         <is>
-          <t>Primary education</t>
+          <t>Youth (ages 15-24)</t>
         </is>
       </c>
     </row>
@@ -25337,12 +25337,12 @@
     <row r="674">
       <c r="A674" t="inlineStr">
         <is>
-          <t>FM.AST.CGOV.ZG.M3</t>
+          <t>FS.AST.CGOV.GD.ZS</t>
         </is>
       </c>
       <c r="B674" t="inlineStr">
         <is>
-          <t>Claims on central government (annual growth as % of broad money)</t>
+          <t>Claims on central government, etc. (% GDP)</t>
         </is>
       </c>
       <c r="C674" t="inlineStr">
@@ -25374,12 +25374,12 @@
     <row r="675">
       <c r="A675" t="inlineStr">
         <is>
-          <t>FS.AST.CGOV.GD.ZS</t>
+          <t>FS.AST.DOMS.GD.ZS</t>
         </is>
       </c>
       <c r="B675" t="inlineStr">
         <is>
-          <t>Claims on central government, etc. (% GDP)</t>
+          <t>Domestic credit provided by financial sector (% of GDP)</t>
         </is>
       </c>
       <c r="C675" t="inlineStr">
@@ -25404,19 +25404,19 @@
       </c>
       <c r="G675" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>Domestic</t>
         </is>
       </c>
     </row>
     <row r="676">
       <c r="A676" t="inlineStr">
         <is>
-          <t>FS.AST.DOMS.GD.ZS</t>
+          <t>FS.AST.DOMO.GD.ZS</t>
         </is>
       </c>
       <c r="B676" t="inlineStr">
         <is>
-          <t>Domestic credit provided by financial sector (% of GDP)</t>
+          <t>Claims on other sectors of the domestic economy (% of GDP)</t>
         </is>
       </c>
       <c r="C676" t="inlineStr">
@@ -25441,19 +25441,19 @@
       </c>
       <c r="G676" t="inlineStr">
         <is>
-          <t>Domestic</t>
+          <t>Other domestic sectors</t>
         </is>
       </c>
     </row>
     <row r="677">
       <c r="A677" t="inlineStr">
         <is>
-          <t>FM.AST.DOMS.CN</t>
+          <t>FS.AST.PRVT.GD.ZS</t>
         </is>
       </c>
       <c r="B677" t="inlineStr">
         <is>
-          <t>Net domestic credit (current LCU)</t>
+          <t>Domestic credit to private sector (% of GDP)</t>
         </is>
       </c>
       <c r="C677" t="inlineStr">
@@ -25478,19 +25478,19 @@
       </c>
       <c r="G677" t="inlineStr">
         <is>
-          <t>Domestic</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
     <row r="678">
       <c r="A678" t="inlineStr">
         <is>
-          <t>FM.AST.NFRG.CN</t>
+          <t>FB.BNK.CAPA.ZS</t>
         </is>
       </c>
       <c r="B678" t="inlineStr">
         <is>
-          <t>Net foreign assets (current LCU)</t>
+          <t>Bank capital to assets ratio (%)</t>
         </is>
       </c>
       <c r="C678" t="inlineStr">
@@ -25510,12 +25510,12 @@
       </c>
       <c r="F678" t="inlineStr">
         <is>
-          <t>Asset</t>
+          <t>Bank</t>
         </is>
       </c>
       <c r="G678" t="inlineStr">
         <is>
-          <t>Net foreign</t>
+          <t>Capital to assets</t>
         </is>
       </c>
     </row>
@@ -25547,7 +25547,7 @@
       </c>
       <c r="F679" t="inlineStr">
         <is>
-          <t>Asset</t>
+          <t>Bank (miscellaneous)</t>
         </is>
       </c>
       <c r="G679" t="inlineStr">
@@ -25559,12 +25559,12 @@
     <row r="680">
       <c r="A680" t="inlineStr">
         <is>
-          <t>FS.AST.DOMO.GD.ZS</t>
+          <t>FD.AST.PRVT.GD.ZS</t>
         </is>
       </c>
       <c r="B680" t="inlineStr">
         <is>
-          <t>Claims on other sectors of the domestic economy (% of GDP)</t>
+          <t>Domestic credit to private sector by banks (% of GDP)</t>
         </is>
       </c>
       <c r="C680" t="inlineStr">
@@ -25584,24 +25584,24 @@
       </c>
       <c r="F680" t="inlineStr">
         <is>
-          <t>Asset</t>
+          <t>Deposit money banks</t>
         </is>
       </c>
       <c r="G680" t="inlineStr">
         <is>
-          <t>Other domestic sectors</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
     <row r="681">
       <c r="A681" t="inlineStr">
         <is>
-          <t>FM.AST.DOMO.ZG.M3</t>
+          <t>FM.AST.CGOV.ZG.M3</t>
         </is>
       </c>
       <c r="B681" t="inlineStr">
         <is>
-          <t>Claims on other sectors of the domestic economy (annual growth as % of broad money)</t>
+          <t>Claims on central government (annual growth as % of broad money)</t>
         </is>
       </c>
       <c r="C681" t="inlineStr">
@@ -25621,24 +25621,24 @@
       </c>
       <c r="F681" t="inlineStr">
         <is>
-          <t>Asset</t>
+          <t>Monetary Survey</t>
         </is>
       </c>
       <c r="G681" t="inlineStr">
         <is>
-          <t>Other domestic sectors</t>
+          <t>Central government</t>
         </is>
       </c>
     </row>
     <row r="682">
       <c r="A682" t="inlineStr">
         <is>
-          <t>FM.AST.PRVT.GD.ZS</t>
+          <t>FM.AST.DOMS.CN</t>
         </is>
       </c>
       <c r="B682" t="inlineStr">
         <is>
-          <t>Monetary Sector credit to private sector (% GDP)</t>
+          <t>Net domestic credit (current LCU)</t>
         </is>
       </c>
       <c r="C682" t="inlineStr">
@@ -25658,24 +25658,24 @@
       </c>
       <c r="F682" t="inlineStr">
         <is>
-          <t>Asset</t>
+          <t>Monetary Survey</t>
         </is>
       </c>
       <c r="G682" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Domestic</t>
         </is>
       </c>
     </row>
     <row r="683">
       <c r="A683" t="inlineStr">
         <is>
-          <t>FM.AST.PRVT.ZG.M3</t>
+          <t>FM.AST.NFRG.CN</t>
         </is>
       </c>
       <c r="B683" t="inlineStr">
         <is>
-          <t>Claims on private sector (annual growth as % of broad money)</t>
+          <t>Net foreign assets (current LCU)</t>
         </is>
       </c>
       <c r="C683" t="inlineStr">
@@ -25695,24 +25695,24 @@
       </c>
       <c r="F683" t="inlineStr">
         <is>
-          <t>Asset</t>
+          <t>Monetary Survey</t>
         </is>
       </c>
       <c r="G683" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Net foreign</t>
         </is>
       </c>
     </row>
     <row r="684">
       <c r="A684" t="inlineStr">
         <is>
-          <t>FS.AST.PRVT.GD.ZS</t>
+          <t>FM.AST.DOMO.ZG.M3</t>
         </is>
       </c>
       <c r="B684" t="inlineStr">
         <is>
-          <t>Domestic credit to private sector (% of GDP)</t>
+          <t>Claims on other sectors of the domestic economy (annual growth as % of broad money)</t>
         </is>
       </c>
       <c r="C684" t="inlineStr">
@@ -25732,24 +25732,24 @@
       </c>
       <c r="F684" t="inlineStr">
         <is>
-          <t>Asset</t>
+          <t>Monetary Survey</t>
         </is>
       </c>
       <c r="G684" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Other domestic sectors</t>
         </is>
       </c>
     </row>
     <row r="685">
       <c r="A685" t="inlineStr">
         <is>
-          <t>FD.AST.PRVT.GD.ZS</t>
+          <t>FM.AST.PRVT.GD.ZS</t>
         </is>
       </c>
       <c r="B685" t="inlineStr">
         <is>
-          <t>Domestic credit to private sector by banks (% of GDP)</t>
+          <t>Monetary Sector credit to private sector (% GDP)</t>
         </is>
       </c>
       <c r="C685" t="inlineStr">
@@ -25769,7 +25769,7 @@
       </c>
       <c r="F685" t="inlineStr">
         <is>
-          <t>Asset</t>
+          <t>Monetary Survey</t>
         </is>
       </c>
       <c r="G685" t="inlineStr">
@@ -25781,12 +25781,12 @@
     <row r="686">
       <c r="A686" t="inlineStr">
         <is>
-          <t>FB.BNK.CAPA.ZS</t>
+          <t>FM.AST.PRVT.ZG.M3</t>
         </is>
       </c>
       <c r="B686" t="inlineStr">
         <is>
-          <t>Bank capital to assets ratio (%)</t>
+          <t>Claims on private sector (annual growth as % of broad money)</t>
         </is>
       </c>
       <c r="C686" t="inlineStr">
@@ -25806,12 +25806,12 @@
       </c>
       <c r="F686" t="inlineStr">
         <is>
-          <t>Bank</t>
+          <t>Monetary Survey</t>
         </is>
       </c>
       <c r="G686" t="inlineStr">
         <is>
-          <t>Capital to assets</t>
+          <t>Private</t>
         </is>
       </c>
     </row>

</xml_diff>